<commit_message>
ultimas actualizaciones reunión miercoles
</commit_message>
<xml_diff>
--- a/flaskr/static/services.xlsx
+++ b/flaskr/static/services.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\roise\Documents\Apam ciber\risk-meter - V2\flaskr\static\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9742D3F1-5D4B-41F1-A05F-7CFBF3E55AF3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{48975194-C140-402A-AD41-D2792988B5E8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Privacy values median" sheetId="1" r:id="rId1"/>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="67" uniqueCount="48">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="67" uniqueCount="49">
   <si>
     <t>Risk dimension</t>
   </si>
@@ -150,37 +150,40 @@
     <t>lud</t>
   </si>
   <si>
-    <t>Digital tool</t>
-  </si>
-  <si>
     <t>OpenAI</t>
-  </si>
-  <si>
-    <t>Email</t>
   </si>
   <si>
     <t>Google</t>
   </si>
   <si>
-    <t>Finance</t>
-  </si>
-  <si>
     <t>Meta</t>
   </si>
   <si>
-    <t>Service A</t>
+    <t>Digital tool service</t>
   </si>
   <si>
-    <t>Service B</t>
+    <t>Email service</t>
   </si>
   <si>
-    <t>Service C</t>
+    <t>Finance service</t>
   </si>
   <si>
-    <t>Service D</t>
+    <t>Social network service B</t>
   </si>
   <si>
-    <t>Service E</t>
+    <t>Social network service A</t>
+  </si>
+  <si>
+    <t>The service has a subscription and collects minimal personal data such as name, surname, and telephone number, also it stores personal messages</t>
+  </si>
+  <si>
+    <t>The service has a subscription and collects minimal personal data such as name, surname, and email</t>
+  </si>
+  <si>
+    <t>The service stores money and collects multiple personal data such as name, surname, and telephone number and address</t>
+  </si>
+  <si>
+    <t>The service  collects personal data such as name, surname, and telephone number, also it stores personal messages</t>
   </si>
 </sst>
 </file>
@@ -2024,13 +2027,13 @@
       <pane xSplit="3" ySplit="1" topLeftCell="D2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="D1" sqref="D1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="A7" sqref="A7"/>
+      <selection pane="bottomRight" activeCell="B6" sqref="B6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="12.85546875" customWidth="1"/>
-    <col min="2" max="2" width="9.85546875" customWidth="1"/>
+    <col min="1" max="1" width="22.85546875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="10.7109375" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="11" hidden="1" customWidth="1"/>
     <col min="4" max="4" width="9.140625" customWidth="1"/>
     <col min="5" max="5" width="11" customWidth="1"/>
@@ -2173,13 +2176,13 @@
     </row>
     <row r="2" spans="1:62" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
-        <v>43</v>
+        <v>40</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>37</v>
+        <v>46</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="D2" s="2">
         <v>12</v>
@@ -2259,13 +2262,13 @@
     </row>
     <row r="3" spans="1:62" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
-        <v>44</v>
+        <v>41</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>39</v>
+        <v>45</v>
       </c>
       <c r="C3" s="2" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="D3" s="2">
         <v>8</v>
@@ -2357,10 +2360,10 @@
     </row>
     <row r="4" spans="1:62" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="2" t="s">
-        <v>45</v>
+        <v>42</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>41</v>
+        <v>47</v>
       </c>
       <c r="C4" s="4"/>
       <c r="D4" s="2">
@@ -2453,13 +2456,13 @@
     </row>
     <row r="5" spans="1:62" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" s="2" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>19</v>
+        <v>48</v>
       </c>
       <c r="C5" s="2" t="s">
-        <v>42</v>
+        <v>39</v>
       </c>
       <c r="D5" s="2">
         <v>6</v>
@@ -2545,10 +2548,10 @@
     </row>
     <row r="6" spans="1:62" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="2" t="s">
-        <v>47</v>
+        <v>43</v>
       </c>
       <c r="B6" s="2" t="s">
-        <v>19</v>
+        <v>48</v>
       </c>
       <c r="C6" s="4"/>
       <c r="D6" s="2">

</xml_diff>

<commit_message>
update new setup and languages
</commit_message>
<xml_diff>
--- a/flaskr/static/services.xlsx
+++ b/flaskr/static/services.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\roise\Documents\Apam ciber\risk-meter - V2\flaskr\static\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{48975194-C140-402A-AD41-D2792988B5E8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4F30042E-A911-4094-A149-4EB252243926}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Privacy values median" sheetId="1" r:id="rId1"/>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="67" uniqueCount="49">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="70" uniqueCount="52">
   <si>
     <t>Risk dimension</t>
   </si>
@@ -184,6 +184,15 @@
   </si>
   <si>
     <t>The service  collects personal data such as name, surname, and telephone number, also it stores personal messages</t>
+  </si>
+  <si>
+    <t>Worst service</t>
+  </si>
+  <si>
+    <t>This service  stores all types of data</t>
+  </si>
+  <si>
+    <t>luds</t>
   </si>
 </sst>
 </file>
@@ -332,7 +341,7 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{00000000-000C-0000-FFFF-FFFF00000000}" name="Table_1" displayName="Table_1" ref="A1:X6">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{00000000-000C-0000-FFFF-FFFF00000000}" name="Table_1" displayName="Table_1" ref="A1:X7">
   <tableColumns count="24">
     <tableColumn id="1" xr3:uid="{00000000-0010-0000-0000-000001000000}" name="Website"/>
     <tableColumn id="2" xr3:uid="{00000000-0010-0000-0000-000002000000}" name="Type"/>
@@ -2027,7 +2036,7 @@
       <pane xSplit="3" ySplit="1" topLeftCell="D2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="D1" sqref="D1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="B6" sqref="B6"/>
+      <selection pane="bottomRight" activeCell="Y9" sqref="Y9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -2629,30 +2638,72 @@
       <c r="BJ6" s="6"/>
     </row>
     <row r="7" spans="1:62" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="4"/>
-      <c r="B7" s="4"/>
+      <c r="A7" s="4" t="s">
+        <v>49</v>
+      </c>
+      <c r="B7" s="4" t="s">
+        <v>50</v>
+      </c>
       <c r="C7" s="4"/>
-      <c r="D7" s="4"/>
-      <c r="E7" s="4"/>
+      <c r="D7" s="4">
+        <v>1</v>
+      </c>
+      <c r="E7" s="4" t="s">
+        <v>51</v>
+      </c>
       <c r="F7" s="4"/>
       <c r="G7" s="4"/>
-      <c r="H7" s="4"/>
-      <c r="I7" s="4"/>
-      <c r="J7" s="4"/>
-      <c r="K7" s="4"/>
-      <c r="L7" s="4"/>
-      <c r="M7" s="4"/>
-      <c r="N7" s="4"/>
-      <c r="O7" s="4"/>
-      <c r="P7" s="2"/>
-      <c r="Q7" s="4"/>
-      <c r="R7" s="4"/>
-      <c r="S7" s="4"/>
-      <c r="T7" s="4"/>
-      <c r="U7" s="4"/>
-      <c r="V7" s="4"/>
-      <c r="W7" s="4"/>
-      <c r="X7" s="4"/>
+      <c r="H7" s="4">
+        <v>1</v>
+      </c>
+      <c r="I7" s="4">
+        <v>1</v>
+      </c>
+      <c r="J7" s="4">
+        <v>1</v>
+      </c>
+      <c r="K7" s="4">
+        <v>1</v>
+      </c>
+      <c r="L7" s="4">
+        <v>1</v>
+      </c>
+      <c r="M7" s="4">
+        <v>1</v>
+      </c>
+      <c r="N7" s="4">
+        <v>1</v>
+      </c>
+      <c r="O7" s="4">
+        <v>1</v>
+      </c>
+      <c r="P7" s="2">
+        <v>1</v>
+      </c>
+      <c r="Q7" s="4">
+        <v>1</v>
+      </c>
+      <c r="R7" s="4">
+        <v>1</v>
+      </c>
+      <c r="S7" s="4">
+        <v>1</v>
+      </c>
+      <c r="T7" s="4">
+        <v>1</v>
+      </c>
+      <c r="U7" s="4">
+        <v>1</v>
+      </c>
+      <c r="V7" s="4">
+        <v>1</v>
+      </c>
+      <c r="W7" s="4">
+        <v>1</v>
+      </c>
+      <c r="X7" s="4">
+        <v>1</v>
+      </c>
       <c r="Y7" s="6"/>
       <c r="Z7" s="6"/>
       <c r="AA7" s="6"/>

</xml_diff>